<commit_message>
update lecture 6 and 7
</commit_message>
<xml_diff>
--- a/schedule2024.xlsx
+++ b/schedule2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d9648ccaee313cb/Documents/DataHandling/datahandling-lecture2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d9648ccaee313cb/Documents/DataHandling/datahandling-lecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{0F3EC862-54C9-4A4E-8BB3-2D44CC95C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB604122-A426-4D01-8B9F-7F59E5308DC3}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{0F3EC862-54C9-4A4E-8BB3-2D44CC95C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C96941C0-447F-4CD1-9C69-AF21A022561D}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="38700" windowHeight="15285" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="624" yWindow="1980" windowWidth="21900" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_2" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>An introduction to data and data processing</t>
   </si>
   <si>
-    <t>M: Ma chapter 3, WiGr chapter 1; C: Mu chapter 2.</t>
-  </si>
-  <si>
     <t>Data storage and data structures</t>
   </si>
   <si>
@@ -93,12 +90,6 @@
     <t>Exercises/Workshop 2: Data storage and data structures</t>
   </si>
   <si>
-    <t>M: Ma chapter 5-7, C: Mu chapter 5.5, Webb et al. (2020), Gentzkow et al. (2019)</t>
-  </si>
-  <si>
-    <t>M: Ma chapter 8, WiGr chapter 11; C: Mu chapter 9.7</t>
-  </si>
-  <si>
     <t>Exercises/Workshop 3: Web data, text, and images</t>
   </si>
   <si>
@@ -108,9 +99,6 @@
     <t>Data preparation and manipulation</t>
   </si>
   <si>
-    <t>M: Ma chapter 9, WiGr chapter 5; C: Mu chapter 9.8</t>
-  </si>
-  <si>
     <t>Basic statistics and data analysis with R</t>
   </si>
   <si>
@@ -123,9 +111,6 @@
     <t>Andrea Burro</t>
   </si>
   <si>
-    <t>M: Ma chapter 12, C: Wickham (2016), Mu chapter 9.10.</t>
-  </si>
-  <si>
     <t>Exercises/Workshop 5: Data preparation and applied data analysis with R</t>
   </si>
   <si>
@@ -141,9 +126,6 @@
     <t>Aurélien Sallin, Andrea Burro</t>
   </si>
   <si>
-    <t>M: Ma chapter 2, WiGr chapters 4 and 6, C: Mu chapter 9.11</t>
-  </si>
-  <si>
     <t>19.09.2024</t>
   </si>
   <si>
@@ -217,6 +199,24 @@
   </si>
   <si>
     <t>Analytics, more visualisation, and data products</t>
+  </si>
+  <si>
+    <t>M: Ma chapter 2, R4DS chapters 2 and 6, C: Mu chapter 9.11</t>
+  </si>
+  <si>
+    <t>M: Ma chapter 3, R4DS chapter 1; C: Mu chapter 2.</t>
+  </si>
+  <si>
+    <t>M: Ma chapter 5-7, 8.5, R4DS chapter 7; C: Mu chapter 5.5, Webb et al. (2020), Gentzkow et al. (2019)</t>
+  </si>
+  <si>
+    <t>M: Ma chapter 8.1-8.4, C: Mu chapter 9.7</t>
+  </si>
+  <si>
+    <t>M: Ma chapter 9, R4DS chapter 3; C: Mu chapter 9.8</t>
+  </si>
+  <si>
+    <t>M: Ma chapter 12, R4DS Chapter 9-11, Mu chapter 9.10.</t>
   </si>
 </sst>
 </file>
@@ -1240,10 +1240,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1511,19 +1507,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="67.140625" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1"/>
-    <col min="7" max="7" width="49.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="67.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" customWidth="1"/>
+    <col min="7" max="7" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1546,9 +1542,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
@@ -1563,15 +1559,15 @@
         <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>7</v>
@@ -1589,12 +1585,12 @@
         <v>13</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>14</v>
@@ -1603,19 +1599,19 @@
         <v>15</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G4" s="29"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
@@ -1633,12 +1629,12 @@
         <v>13</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>7</v>
@@ -1650,18 +1646,18 @@
         <v>9</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>14</v>
@@ -1673,16 +1669,16 @@
         <v>16</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>7</v>
@@ -1694,18 +1690,18 @@
         <v>9</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>7</v>
@@ -1717,18 +1713,18 @@
         <v>9</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>14</v>
@@ -1740,42 +1736,42 @@
         <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="15"/>
       <c r="E11" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
       <c r="E12" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>7</v>
@@ -1787,18 +1783,18 @@
         <v>9</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>7</v>
@@ -1810,18 +1806,18 @@
         <v>9</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>14</v>
@@ -1833,16 +1829,16 @@
         <v>16</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>7</v>
@@ -1854,18 +1850,18 @@
         <v>9</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>7</v>
@@ -1877,18 +1873,16 @@
         <v>9</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>14</v>
@@ -1900,16 +1894,16 @@
         <v>16</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>7</v>
@@ -1921,16 +1915,18 @@
         <v>9</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>7</v>
@@ -1942,16 +1938,15 @@
         <v>9</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>14</v>
@@ -1963,16 +1958,16 @@
         <v>16</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>14</v>
@@ -1981,17 +1976,17 @@
         <v>15</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="21"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" s="7"/>
     </row>
   </sheetData>

</xml_diff>